<commit_message>
Coding web scraper for speeches
</commit_message>
<xml_diff>
--- a/Descriptive stats (corrected).xlsx
+++ b/Descriptive stats (corrected).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Honours-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A879BE-7AA5-461A-A0F5-C48E2EB635D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C03E91-D6E3-4F5A-8F3F-90F625BA9DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1232,1017 +1232,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>sheet1!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Net negativity score with unemploy</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>sheet1!$A$2:$A$161</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="160"/>
-                <c:pt idx="0">
-                  <c:v>38993</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>39028</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>39056</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39119</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39147</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>39175</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>39203</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39238</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>39266</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>39301</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>39329</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>39357</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>39392</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>39420</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>39483</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>39511</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>39539</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>39574</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>39602</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>39630</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>39665</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>39693</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>39728</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>39756</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>39784</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>39847</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>39875</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>39910</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>39938</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>39966</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>40001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>40029</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>40057</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>40092</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>40120</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>40148</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>40211</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>40239</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>40274</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40302</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40330</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>40365</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>40393</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>40428</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>40456</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>40484</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>40519</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>40575</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>40603</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>40638</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>40666</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>40701</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>40729</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>40757</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>40792</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>40820</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>40848</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>40883</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>40946</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>40974</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>41002</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>41030</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>41065</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>41093</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>41128</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>41156</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>41184</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>41219</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>41247</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>41310</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>41338</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>41366</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>41401</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>41429</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>41457</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>41492</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>41520</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>41548</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>41583</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>41611</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>41674</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>41702</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>41730</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>41765</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>41793</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>41821</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>41856</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>41884</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>41919</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>41947</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>41975</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>42038</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>42066</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>42101</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>42129</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>42157</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>42192</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>42220</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>42248</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>42283</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>42311</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>42339</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>42402</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>42430</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>42465</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>42493</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>42528</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>42556</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>42584</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>42619</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>42647</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>42675</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>42710</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>42773</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>42801</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>42829</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>42857</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>42892</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>42920</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>42948</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>42983</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>43011</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>43046</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>43074</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>43137</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>43165</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>43193</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>43221</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>43256</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>43284</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>43319</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>43347</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>43375</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>43410</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>43438</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>43501</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>43529</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>43557</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>43592</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>43620</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>43648</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>43683</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>43711</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>43739</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>43774</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>43802</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>43865</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>43893</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>43908</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>43928</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>43956</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>43984</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>44019</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>44047</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>44075</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>44110</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>44138</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>44166</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>44229</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>44257</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>sheet1!$H$2:$H$161</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="160"/>
-                <c:pt idx="0">
-                  <c:v>1.7190278601066981E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.8154311649016638E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.5080385852090031E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4981273408239701E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.6730637422892389E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.5187969924812026E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.528239202657807E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1.364256480218281E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.4444444444444436E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0024271844660199E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.695813460519343E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.6245487364620941E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.9382716049382724E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8659295093296471E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.166489925768823E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.1981806367771277E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.5384615384615391E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.3076923076923082E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.2091038406827881E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.8121170864533697E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.9736247174076868E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.5702331141661681E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.0829320492241842E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.9049235993208829E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.814258911819887E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.43622597553873E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.0895334174022699E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.2342064714946069E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.2804097311139561E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.293396868618108E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-8.708272859216255E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-1.08153078202995E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-3.4246575342465752E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7.7821011673151752E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>8.2236842105263153E-4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7.2306579898770787E-4</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.4271211022480053E-3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.4435261707988982E-3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-8.7912087912087912E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>5.2592036063110444E-3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.847745750184775E-2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.345609065155807E-2</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6.313131313131313E-3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>-3.2894736842105261E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>8.8919288645690833E-3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.8564356435643559E-3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>-3.3222591362126251E-3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2.569043031470777E-3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>5.8309037900874626E-3</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>6.0553633217993079E-3</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3.9973351099267156E-3</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1.6962220508866619E-2</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1.6141429669485011E-2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2.1446078431372549E-2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2.0266666666666669E-2</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1.9147621988882021E-2</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5.3349140486069948E-3</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>2.1097046413502109E-2</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1.9595035924232528E-3</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1.9081272084805659E-2</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1.987767584097859E-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2.2808267997148971E-2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3.8102643856920693E-2</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1.3582342954159591E-2</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>2.5434243176178661E-2</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>2.3809523809523812E-2</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1.5873015873015869E-2</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>8.5178875638841568E-4</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1.5819209039548018E-2</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>-6.9637883008356546E-4</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>5.3333333333333332E-3</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7.0422535211267609E-4</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1.3061224489795921E-2</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>2.2260273972602738E-2</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1.535974130962005E-2</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>5.0724637681159417E-3</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>-7.6481835564053526E-3</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1.0769230769230771E-2</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>-3.3726812816188868E-3</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>-6.5502183406113534E-3</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1.5129682997118161E-2</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8.3542188805346695E-3</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>6.9659442724458202E-3</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1.0371650821089019E-2</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1.9667170953101359E-2</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>1.4035087719298249E-2</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>1.2648221343873519E-2</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>1.8072289156626509E-2</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1.7123287671232879E-2</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>1.8502943650126159E-2</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>1.2145748987854249E-2</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>6.3734862970044612E-4</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1.5968063872255491E-2</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>1.723076923076923E-2</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1.2408759124087589E-2</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>5.5521283158544111E-3</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>4.8989589712186161E-3</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>1.5852047556142671E-2</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>8.1199250468457218E-3</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>1.9852524106636411E-2</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>1.6641452344931921E-2</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>2.0262869660460019E-2</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>3.1027795733678091E-2</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>8.9736399326977006E-3</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>1.2544802867383509E-2</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>2.0484171322160152E-2</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>1.904136572554169E-2</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>2.0207536865101041E-2</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>1.5882352941176469E-2</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>5.3821313240043061E-3</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>6.2500000000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>2.046384720327421E-3</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>1.1820330969267139E-3</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>-4.8780487804878049E-3</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>-2.6343519494204421E-3</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>7.4074074074074077E-3</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>-6.4705882352941177E-3</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>1.5831134564643801E-3</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>-1.2121212121212119E-2</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>5.170630816959669E-3</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>2.4975024975024979E-3</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>-4.881025015253203E-3</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>-6.3913470993117007E-3</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>-1.842751842751843E-3</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>-9.372071227741331E-4</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>-2.5075225677031088E-3</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>9.3327111525898267E-3</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>-2.1141649048625789E-3</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>3.2740879326473341E-3</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>4.6728971962616819E-3</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>1.964636542239686E-3</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>9.9739809193408503E-3</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>1.6591251885369529E-2</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>2.8120184899845919E-2</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>3.0032467532467529E-2</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>2.9182079736950271E-2</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>2.301054650047939E-2</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>2.0647583294228059E-2</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>1.3559322033898299E-2</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>1.1701608971233551E-2</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>2.9917250159134309E-2</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>1.9317160826594789E-2</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>1.7209302325581391E-2</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>1.9370460048426151E-2</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>1.996672212978369E-2</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>3.562653562653563E-2</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>8.771929824561403E-3</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>2.5333333333333329E-2</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>3.7529319781078971E-2</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>3.9382650345928687E-2</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>3.8612199216564072E-2</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>2.9912754466140421E-2</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>1.7932489451476789E-2</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>8.2644628099173556E-3</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>-5.8796924468566261E-3</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>5.681818181818182E-3</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>-1.374255611543747E-2</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>-3.3003300330032999E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3542-4104-801D-E60B253BE142}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2254,6 +1243,1041 @@
         <c:smooth val="0"/>
         <c:axId val="1889491280"/>
         <c:axId val="1889487952"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>sheet1!$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Net negativity score with unemploy</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>sheet1!$A$2:$A$161</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="160"/>
+                      <c:pt idx="0">
+                        <c:v>38993</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>39028</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>39056</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>39119</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>39147</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>39175</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>39203</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>39238</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>39266</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>39301</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>39329</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>39357</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>39392</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>39420</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>39483</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>39511</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>39539</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>39574</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>39602</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>39630</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>39665</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>39693</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>39728</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>39756</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>39784</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>39847</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>39875</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>39910</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>39938</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>39966</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>40001</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>40029</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>40057</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>40092</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>40120</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>40148</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>40211</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>40239</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>40274</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>40302</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40330</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>40365</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>40393</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>40428</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>40456</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>40484</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>40519</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>40575</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>40603</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>40638</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>40666</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>40701</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>40729</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>40757</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>40792</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>40820</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>40848</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>40883</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>40946</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>40974</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>41002</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>41030</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>41065</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>41093</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>41128</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>41156</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>41184</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>41219</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>41247</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>41310</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>41338</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>41366</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>41401</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>41429</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>41457</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>41492</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>41520</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>41548</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>41583</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>41611</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>41674</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>41702</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>41730</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>41765</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>41793</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>41821</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>41856</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>41884</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>41919</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>41947</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>41975</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>42038</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>42066</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>42101</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>42129</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>42157</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>42192</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>42220</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>42248</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>42283</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>42311</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>42339</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>42402</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>42430</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>42465</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>42493</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>42528</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>42556</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>42584</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>42619</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>42647</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>42675</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>42710</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>42773</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>42801</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>42829</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>42857</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>42892</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>42920</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>42948</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>42983</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>43011</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>43046</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>43074</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>43137</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>43165</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>43193</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>43221</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>43256</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>43284</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>43319</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>43347</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>43375</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>43410</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>43438</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>43501</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>43529</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>43557</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>43592</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>43620</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>43648</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>43683</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>43711</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>43739</c:v>
+                      </c:pt>
+                      <c:pt idx="144">
+                        <c:v>43774</c:v>
+                      </c:pt>
+                      <c:pt idx="145">
+                        <c:v>43802</c:v>
+                      </c:pt>
+                      <c:pt idx="146">
+                        <c:v>43865</c:v>
+                      </c:pt>
+                      <c:pt idx="147">
+                        <c:v>43893</c:v>
+                      </c:pt>
+                      <c:pt idx="148">
+                        <c:v>43908</c:v>
+                      </c:pt>
+                      <c:pt idx="149">
+                        <c:v>43928</c:v>
+                      </c:pt>
+                      <c:pt idx="150">
+                        <c:v>43956</c:v>
+                      </c:pt>
+                      <c:pt idx="151">
+                        <c:v>43984</c:v>
+                      </c:pt>
+                      <c:pt idx="152">
+                        <c:v>44019</c:v>
+                      </c:pt>
+                      <c:pt idx="153">
+                        <c:v>44047</c:v>
+                      </c:pt>
+                      <c:pt idx="154">
+                        <c:v>44075</c:v>
+                      </c:pt>
+                      <c:pt idx="155">
+                        <c:v>44110</c:v>
+                      </c:pt>
+                      <c:pt idx="156">
+                        <c:v>44138</c:v>
+                      </c:pt>
+                      <c:pt idx="157">
+                        <c:v>44166</c:v>
+                      </c:pt>
+                      <c:pt idx="158">
+                        <c:v>44229</c:v>
+                      </c:pt>
+                      <c:pt idx="159">
+                        <c:v>44257</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>sheet1!$H$2:$H$161</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0%</c:formatCode>
+                      <c:ptCount val="160"/>
+                      <c:pt idx="0">
+                        <c:v>1.7190278601066981E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.8154311649016638E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.5080385852090031E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.4981273408239701E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2.6730637422892389E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>7.5187969924812026E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.528239202657807E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-1.364256480218281E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4.4444444444444436E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2.0024271844660199E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.695813460519343E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1.6245487364620941E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4.9382716049382724E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1.8659295093296471E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>1.166489925768823E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>5.1981806367771277E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.5384615384615391E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>2.3076923076923082E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>1.2091038406827881E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>3.8121170864533697E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>4.9736247174076868E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>2.5702331141661681E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>5.0829320492241842E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>3.9049235993208829E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>2.814258911819887E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>3.43622597553873E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>3.0895334174022699E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>2.2342064714946069E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>1.2804097311139561E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>1.293396868618108E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>-8.708272859216255E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>-1.08153078202995E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>-3.4246575342465752E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>7.7821011673151752E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>8.2236842105263153E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>7.2306579898770787E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>9.4271211022480053E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>3.4435261707988982E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>-8.7912087912087912E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>5.2592036063110444E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>1.847745750184775E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>1.345609065155807E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>6.313131313131313E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>-3.2894736842105261E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>8.8919288645690833E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>1.8564356435643559E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>-3.3222591362126251E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>2.569043031470777E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>5.8309037900874626E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>6.0553633217993079E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>3.9973351099267156E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1.6962220508866619E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>1.6141429669485011E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>2.1446078431372549E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>2.0266666666666669E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>1.9147621988882021E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>5.3349140486069948E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>2.1097046413502109E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>1.9595035924232528E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>1.9081272084805659E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>1.987767584097859E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>2.2808267997148971E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>3.8102643856920693E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>1.3582342954159591E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>2.5434243176178661E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>2.3809523809523812E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>1.5873015873015869E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>8.5178875638841568E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>1.5819209039548018E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>-6.9637883008356546E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>5.3333333333333332E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>7.0422535211267609E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>1.3061224489795921E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>2.2260273972602738E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>1.535974130962005E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>5.0724637681159417E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>-7.6481835564053526E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>1.0769230769230771E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>-3.3726812816188868E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>-6.5502183406113534E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>1.5129682997118161E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>8.3542188805346695E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>6.9659442724458202E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>1.0371650821089019E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>1.9667170953101359E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>1.4035087719298249E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>1.2648221343873519E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>1.8072289156626509E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>1.7123287671232879E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>1.8502943650126159E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>1.2145748987854249E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>6.3734862970044612E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>1.5968063872255491E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>1.723076923076923E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>1.2408759124087589E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>5.5521283158544111E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>4.8989589712186161E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>1.5852047556142671E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>8.1199250468457218E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>1.9852524106636411E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>1.6641452344931921E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>2.0262869660460019E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>3.1027795733678091E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>8.9736399326977006E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>1.2544802867383509E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>2.0484171322160152E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>1.904136572554169E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>2.0207536865101041E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>1.5882352941176469E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>5.3821313240043061E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>6.2500000000000003E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>2.046384720327421E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>1.1820330969267139E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>-4.8780487804878049E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>-2.6343519494204421E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>7.4074074074074077E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>-6.4705882352941177E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>1.5831134564643801E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>-1.2121212121212119E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>5.170630816959669E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>2.4975024975024979E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>-4.881025015253203E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>-6.3913470993117007E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>-1.842751842751843E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>-9.372071227741331E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>-2.5075225677031088E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>9.3327111525898267E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>-2.1141649048625789E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>3.2740879326473341E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>4.6728971962616819E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>1.964636542239686E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>9.9739809193408503E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>1.6591251885369529E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>2.8120184899845919E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>3.0032467532467529E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>2.9182079736950271E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>2.301054650047939E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>2.0647583294228059E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>1.3559322033898299E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>1.1701608971233551E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>2.9917250159134309E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>1.9317160826594789E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="144">
+                        <c:v>1.7209302325581391E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="145">
+                        <c:v>1.9370460048426151E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="146">
+                        <c:v>1.996672212978369E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="147">
+                        <c:v>3.562653562653563E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="148">
+                        <c:v>8.771929824561403E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="149">
+                        <c:v>2.5333333333333329E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="150">
+                        <c:v>3.7529319781078971E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="151">
+                        <c:v>3.9382650345928687E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="152">
+                        <c:v>3.8612199216564072E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="153">
+                        <c:v>2.9912754466140421E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="154">
+                        <c:v>1.7932489451476789E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="155">
+                        <c:v>8.2644628099173556E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="156">
+                        <c:v>-5.8796924468566261E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="157">
+                        <c:v>5.681818181818182E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="158">
+                        <c:v>-1.374255611543747E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="159">
+                        <c:v>-3.3003300330032999E-3</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-3542-4104-801D-E60B253BE142}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:dateAx>
         <c:axId val="1889491280"/>
@@ -2262,6 +2286,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Date	</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -2326,6 +2405,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Percent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2369,37 +2503,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5833,16 +5936,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>124360</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>92363</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>574633</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>46181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>324097</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>158338</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>162461</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>112156</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6283,8 +6386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AM28" sqref="AM28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI24" sqref="AI24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>